<commit_message>
regenerate all outputs using 'make' all after changing schema
</commit_message>
<xml_diff>
--- a/project/excel/datalad_schema.xlsx
+++ b/project/excel/datalad_schema.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dataset" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="DatasetCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="File" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Person" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DatasetCollection" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +428,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -451,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,51 +464,138 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>authors</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>hasPart</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>homepage</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>keywords</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>last-updated</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>checksum_md5</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>path_posix</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>size_in_bytes</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>